<commit_message>
ru: OФ - Invoice
</commit_message>
<xml_diff>
--- a/data/numerator.xlsx
+++ b/data/numerator.xlsx
@@ -208,7 +208,7 @@
     <t xml:space="preserve">Счет-фактура</t>
   </si>
   <si>
-    <t xml:space="preserve">OФ</t>
+    <t xml:space="preserve">ФA</t>
   </si>
   <si>
     <t xml:space="preserve">Оптовый прайс</t>
@@ -470,7 +470,7 @@
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.38"/>

</xml_diff>